<commit_message>
fixed uncertainties of fe11+
</commit_message>
<xml_diff>
--- a/csdata/Fe/SI/Fe0+.xlsx
+++ b/csdata/Fe/SI/Fe0+.xlsx
@@ -1,17 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmondeel/Documents/CfA/Chandra/CHANDRA-Rates/csdata/Fe/SI/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676857CE-34D0-7644-A429-38C7A4D75574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-20" yWindow="780" windowWidth="15120" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Energy (eV)</t>
   </si>
@@ -30,34 +52,49 @@
   <si>
     <t>Multiple ionization of iron by electron impact Shah 1993</t>
   </si>
+  <si>
+    <t>Unc at peak</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -66,58 +103,57 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="165" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -307,20 +343,25 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:F67"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -336,8 +377,11 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2">
+      <c r="F1" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
         <v>8.1</v>
       </c>
@@ -345,29 +389,33 @@
         <v>0.33</v>
       </c>
       <c r="C2" s="5">
-        <v>0.06807672142516853</v>
+        <v>6.8076721425168532E-2</v>
       </c>
       <c r="D2" s="6">
-        <v>-16.0</v>
+        <v>-16</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3">
+      <c r="F2">
+        <f>_xlfn.XLOOKUP(MAX(B:B),B:B,C:C)/MAX(B:B)</f>
+        <v>0.14678680724781407</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
-        <v>8.3</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="B3" s="4">
         <v>0.44</v>
       </c>
       <c r="C3" s="5">
-        <v>0.0859916274994258</v>
+        <v>8.5991627499425793E-2</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>8.6</v>
       </c>
@@ -379,9 +427,9 @@
       </c>
       <c r="D4" s="2"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
-        <v>8.8</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="B5" s="4">
         <v>1.08</v>
@@ -390,7 +438,7 @@
         <v>0.16661764612429264</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>9.4</v>
       </c>
@@ -401,7 +449,7 @@
         <v>0.20394548291148792</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>9.9</v>
       </c>
@@ -412,7 +460,7 @@
         <v>0.22996382324183082</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>10.4</v>
       </c>
@@ -423,31 +471,31 @@
         <v>0.28878254794914465</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="B9" s="4">
-        <v>2.18</v>
+        <v>2.1800000000000002</v>
       </c>
       <c r="C9" s="8">
         <v>0.31551076051380567</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>11.6</v>
       </c>
       <c r="B10" s="4">
-        <v>2.22</v>
+        <v>2.2200000000000002</v>
       </c>
       <c r="C10" s="8">
         <v>0.3185853731733459</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="B11" s="4">
         <v>2.39</v>
@@ -456,7 +504,7 @@
         <v>0.34922365326535376</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>12.6</v>
       </c>
@@ -467,9 +515,9 @@
         <v>0.35862426019442695</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="B13" s="4">
         <v>2.5</v>
@@ -478,9 +526,9 @@
         <v>0.36687872655688286</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="B14" s="4">
         <v>2.83</v>
@@ -489,20 +537,20 @@
         <v>0.41118662429607317</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="B15" s="4">
         <v>2.94</v>
       </c>
       <c r="C15" s="8">
-        <v>0.4260452558121027</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>0.42604525581210267</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
-        <v>16.1</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="B16" s="4">
         <v>3.15</v>
@@ -511,7 +559,7 @@
         <v>0.46268888035050076</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="3">
         <v>16.8</v>
       </c>
@@ -519,45 +567,45 @@
         <v>3.42</v>
       </c>
       <c r="C17" s="8">
-        <v>0.4961344978934644</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>0.49613449789346442</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="3">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="B18" s="4">
         <v>3.65</v>
       </c>
       <c r="C18" s="8">
-        <v>0.5385359783709905</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>0.53853597837099054</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="3">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="B19" s="4">
         <v>3.91</v>
       </c>
       <c r="C19" s="8">
-        <v>0.5675797388913739</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>0.56757973889137392</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="3">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="B20" s="4">
         <v>3.95</v>
       </c>
       <c r="C20" s="8">
-        <v>0.5680748190159463</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>0.56807481901594625</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="3">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="B21" s="4">
         <v>4.01</v>
@@ -566,29 +614,29 @@
         <v>0.5762551171139394</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="3">
-        <v>29.0</v>
+        <v>29</v>
       </c>
       <c r="B22" s="4">
         <v>3.8</v>
       </c>
       <c r="C22" s="8">
-        <v>0.5555393775422225</v>
-      </c>
-    </row>
-    <row r="23">
+        <v>0.55553937754222249</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="3">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="B23" s="4">
         <v>3.92</v>
       </c>
       <c r="C23" s="8">
-        <v>0.5639870920508732</v>
-      </c>
-    </row>
-    <row r="24">
+        <v>0.56398709205087316</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="3">
         <v>32.5</v>
       </c>
@@ -596,483 +644,483 @@
         <v>3.98</v>
       </c>
       <c r="C24" s="8">
-        <v>0.5699752977103482</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="9">
-        <v>35.0</v>
+        <v>0.56997529771034816</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="6">
+        <v>35</v>
       </c>
       <c r="B25" s="4">
         <v>4.08</v>
       </c>
       <c r="C25" s="8">
-        <v>0.5988901735710814</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="9">
-        <v>42.0</v>
+        <v>0.59889017357108143</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="6">
+        <v>42</v>
       </c>
       <c r="B26" s="4">
         <v>3.77</v>
       </c>
       <c r="C26" s="8">
-        <v>0.5487010479304738</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="9">
-        <v>47.0</v>
+        <v>0.54870104793047381</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="6">
+        <v>47</v>
       </c>
       <c r="B27" s="4">
         <v>3.76</v>
       </c>
       <c r="C27" s="8">
-        <v>0.5531699196449495</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="9">
-        <v>52.0</v>
+        <v>0.55316991964494955</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="6">
+        <v>52</v>
       </c>
       <c r="B28" s="4">
         <v>3.58</v>
       </c>
       <c r="C28" s="8">
-        <v>0.5203858568408639</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="9">
-        <v>50.0</v>
-      </c>
-      <c r="B29" s="9">
+        <v>0.52038585684086391</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="6">
+        <v>50</v>
+      </c>
+      <c r="B29" s="6">
         <v>3.42</v>
       </c>
       <c r="C29" s="8">
-        <v>0.5151208013660485</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="9">
-        <v>70.0</v>
-      </c>
-      <c r="B30" s="9">
+        <v>0.51512080136604854</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="6">
+        <v>70</v>
+      </c>
+      <c r="B30" s="6">
         <v>3.29</v>
       </c>
       <c r="C30" s="8">
         <v>0.49452235540974293</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" s="9">
-        <v>80.0</v>
-      </c>
-      <c r="B31" s="9">
+    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="6">
+        <v>80</v>
+      </c>
+      <c r="B31" s="6">
         <v>2.93</v>
       </c>
       <c r="C31" s="8">
-        <v>0.4334328552382711</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="9">
-        <v>85.0</v>
-      </c>
-      <c r="B32" s="9">
+        <v>0.43343285523827108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="6">
+        <v>85</v>
+      </c>
+      <c r="B32" s="6">
         <v>2.93</v>
       </c>
       <c r="C32" s="8">
         <v>0.43030691372554086</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" s="9">
-        <v>90.0</v>
-      </c>
-      <c r="B33" s="9">
+    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="6">
+        <v>90</v>
+      </c>
+      <c r="B33" s="6">
         <v>2.87</v>
       </c>
       <c r="C33" s="8">
-        <v>0.4193366666534183</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="9">
-        <v>95.0</v>
-      </c>
-      <c r="B34" s="9">
+        <v>0.41933666665341829</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="6">
+        <v>95</v>
+      </c>
+      <c r="B34" s="6">
         <v>2.83</v>
       </c>
       <c r="C34" s="8">
         <v>0.4202076153522209</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" s="9">
-        <v>100.0</v>
-      </c>
-      <c r="B35" s="9">
+    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="6">
+        <v>100</v>
+      </c>
+      <c r="B35" s="6">
         <v>2.6</v>
       </c>
       <c r="C35" s="8">
         <v>0.3865177874302812</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" s="9">
-        <v>110.0</v>
-      </c>
-      <c r="B36" s="9">
+    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="6">
+        <v>110</v>
+      </c>
+      <c r="B36" s="6">
         <v>2.46</v>
       </c>
       <c r="C36" s="8">
-        <v>0.3647072250449668</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="9">
-        <v>120.0</v>
-      </c>
-      <c r="B37" s="9">
-        <v>2.51</v>
+        <v>0.36470722504496678</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="6">
+        <v>120</v>
+      </c>
+      <c r="B37" s="6">
+        <v>2.5099999999999998</v>
       </c>
       <c r="C37" s="8">
         <v>0.37467580653145993</v>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" s="9">
-        <v>130.0</v>
-      </c>
-      <c r="B38" s="9">
+    <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="6">
+        <v>130</v>
+      </c>
+      <c r="B38" s="6">
         <v>2.27</v>
       </c>
       <c r="C38" s="8">
         <v>0.34336109272892296</v>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" s="9">
-        <v>140.0</v>
-      </c>
-      <c r="B39" s="9">
+    <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="6">
+        <v>140</v>
+      </c>
+      <c r="B39" s="6">
         <v>2.34</v>
       </c>
       <c r="C39" s="8">
-        <v>0.3455745360989435</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="9">
-        <v>150.0</v>
-      </c>
-      <c r="B40" s="9">
+        <v>0.34557453609894351</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="6">
+        <v>150</v>
+      </c>
+      <c r="B40" s="6">
         <v>2.19</v>
       </c>
       <c r="C40" s="8">
-        <v>0.3195364767909918</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="9">
-        <v>160.0</v>
-      </c>
-      <c r="B41" s="9">
+        <v>0.31953647679099179</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="6">
+        <v>160</v>
+      </c>
+      <c r="B41" s="6">
         <v>2.14</v>
       </c>
       <c r="C41" s="8">
         <v>0.31915538535327903</v>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" s="9">
-        <v>170.0</v>
-      </c>
-      <c r="B42" s="9">
+    <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="6">
+        <v>170</v>
+      </c>
+      <c r="B42" s="6">
         <v>1.97</v>
       </c>
       <c r="C42" s="8">
-        <v>0.2933694598965612</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="9">
-        <v>180.0</v>
-      </c>
-      <c r="B43" s="9">
+        <v>0.29336945989656121</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="6">
+        <v>180</v>
+      </c>
+      <c r="B43" s="6">
         <v>1.92</v>
       </c>
       <c r="C43" s="8">
-        <v>0.2804522062669503</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="9">
-        <v>190.0</v>
-      </c>
-      <c r="B44" s="9">
+        <v>0.28045220626695028</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="6">
+        <v>190</v>
+      </c>
+      <c r="B44" s="6">
         <v>1.84</v>
       </c>
       <c r="C44" s="8">
-        <v>0.266941491716818</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="9">
-        <v>200.0</v>
-      </c>
-      <c r="B45" s="9">
+        <v>0.26694149171681802</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="6">
+        <v>200</v>
+      </c>
+      <c r="B45" s="6">
         <v>1.82</v>
       </c>
       <c r="C45" s="8">
         <v>0.27022775579129543</v>
       </c>
     </row>
-    <row r="46">
-      <c r="A46" s="9">
-        <v>225.0</v>
-      </c>
-      <c r="B46" s="9">
+    <row r="46" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="6">
+        <v>225</v>
+      </c>
+      <c r="B46" s="6">
         <v>1.7</v>
       </c>
       <c r="C46" s="8">
         <v>0.25108564275959705</v>
       </c>
     </row>
-    <row r="47">
-      <c r="A47" s="9">
-        <v>250.0</v>
-      </c>
-      <c r="B47" s="9">
+    <row r="47" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="6">
+        <v>250</v>
+      </c>
+      <c r="B47" s="6">
         <v>1.68</v>
       </c>
       <c r="C47" s="8">
-        <v>0.2518313721520812</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="9">
-        <v>275.0</v>
-      </c>
-      <c r="B48" s="9">
+        <v>0.25183137215208118</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="6">
+        <v>275</v>
+      </c>
+      <c r="B48" s="6">
         <v>1.53</v>
       </c>
       <c r="C48" s="8">
         <v>0.22534782004714404</v>
       </c>
     </row>
-    <row r="49">
-      <c r="A49" s="9">
-        <v>300.0</v>
-      </c>
-      <c r="B49" s="9">
+    <row r="49" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A49" s="6">
+        <v>300</v>
+      </c>
+      <c r="B49" s="6">
         <v>1.46</v>
       </c>
       <c r="C49" s="8">
-        <v>0.2160540673072368</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="9">
-        <v>325.0</v>
-      </c>
-      <c r="B50" s="9">
+        <v>0.21605406730723681</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="A50" s="6">
+        <v>325</v>
+      </c>
+      <c r="B50" s="6">
         <v>1.35</v>
       </c>
       <c r="C50" s="8">
         <v>0.2015465206844316</v>
       </c>
     </row>
-    <row r="51">
-      <c r="A51" s="9">
-        <v>370.0</v>
-      </c>
-      <c r="B51" s="9">
+    <row r="51" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="A51" s="6">
+        <v>370</v>
+      </c>
+      <c r="B51" s="6">
         <v>1.3</v>
       </c>
       <c r="C51" s="8">
-        <v>0.1949974358805777</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="9">
-        <v>400.0</v>
-      </c>
-      <c r="B52" s="9">
-        <v>1.12</v>
+        <v>0.19499743588057769</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="A52" s="6">
+        <v>400</v>
+      </c>
+      <c r="B52" s="6">
+        <v>1.1200000000000001</v>
       </c>
       <c r="C52" s="8">
         <v>0.16457897800144466</v>
       </c>
     </row>
-    <row r="53">
-      <c r="A53" s="9">
-        <v>450.0</v>
-      </c>
-      <c r="B53" s="9">
+    <row r="53" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="A53" s="6">
+        <v>450</v>
+      </c>
+      <c r="B53" s="6">
         <v>1.05</v>
       </c>
       <c r="C53" s="8">
         <v>0.1552707313050338</v>
       </c>
     </row>
-    <row r="54">
-      <c r="A54" s="9">
-        <v>500.0</v>
-      </c>
-      <c r="B54" s="9">
+    <row r="54" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="A54" s="6">
+        <v>500</v>
+      </c>
+      <c r="B54" s="6">
         <v>1.06</v>
       </c>
       <c r="C54" s="8">
         <v>0.16007048447480882</v>
       </c>
     </row>
-    <row r="55">
-      <c r="A55" s="9">
-        <v>550.0</v>
-      </c>
-      <c r="B55" s="9">
+    <row r="55" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="A55" s="6">
+        <v>550</v>
+      </c>
+      <c r="B55" s="6">
         <v>0.91</v>
       </c>
       <c r="C55" s="8">
         <v>0.13353186885534107</v>
       </c>
     </row>
-    <row r="56">
-      <c r="A56" s="9">
-        <v>600.0</v>
-      </c>
-      <c r="B56" s="9">
+    <row r="56" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="A56" s="6">
+        <v>600</v>
+      </c>
+      <c r="B56" s="6">
         <v>0.87</v>
       </c>
       <c r="C56" s="8">
         <v>0.12544018494884326</v>
       </c>
     </row>
-    <row r="57">
-      <c r="A57" s="9">
-        <v>650.0</v>
-      </c>
-      <c r="B57" s="9">
+    <row r="57" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="A57" s="6">
+        <v>650</v>
+      </c>
+      <c r="B57" s="6">
         <v>0.82</v>
       </c>
       <c r="C57" s="8">
         <v>0.12156907501498891</v>
       </c>
     </row>
-    <row r="58">
-      <c r="A58" s="9">
-        <v>710.0</v>
-      </c>
-      <c r="B58" s="9">
+    <row r="58" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="A58" s="6">
+        <v>710</v>
+      </c>
+      <c r="B58" s="6">
         <v>0.77</v>
       </c>
       <c r="C58" s="8">
         <v>0.11189655937516578</v>
       </c>
     </row>
-    <row r="59">
-      <c r="A59" s="9">
-        <v>760.0</v>
-      </c>
-      <c r="B59" s="9">
+    <row r="59" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="A59" s="6">
+        <v>760</v>
+      </c>
+      <c r="B59" s="6">
         <v>0.75</v>
       </c>
       <c r="C59" s="8">
         <v>0.11236102527122117</v>
       </c>
     </row>
-    <row r="60">
-      <c r="A60" s="9">
-        <v>800.0</v>
-      </c>
-      <c r="B60" s="9">
+    <row r="60" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="A60" s="6">
+        <v>800</v>
+      </c>
+      <c r="B60" s="6">
         <v>0.7</v>
       </c>
       <c r="C60" s="8">
         <v>0.10584894897919395</v>
       </c>
     </row>
-    <row r="61">
-      <c r="A61" s="9">
-        <v>830.0</v>
-      </c>
-      <c r="B61" s="9">
+    <row r="61" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="A61" s="6">
+        <v>830</v>
+      </c>
+      <c r="B61" s="6">
         <v>0.7</v>
       </c>
       <c r="C61" s="8">
         <v>0.10584894897919395</v>
       </c>
     </row>
-    <row r="62">
-      <c r="A62" s="9">
-        <v>860.0</v>
-      </c>
-      <c r="B62" s="9">
+    <row r="62" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="A62" s="6">
+        <v>860</v>
+      </c>
+      <c r="B62" s="6">
         <v>0.68</v>
       </c>
       <c r="C62" s="8">
         <v>0.10326199688171832</v>
       </c>
     </row>
-    <row r="63">
-      <c r="A63" s="9">
-        <v>900.0</v>
-      </c>
-      <c r="B63" s="9">
+    <row r="63" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="A63" s="6">
+        <v>900</v>
+      </c>
+      <c r="B63" s="6">
         <v>0.65</v>
       </c>
       <c r="C63" s="8">
-        <v>0.0994032192637643</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" s="9">
-        <v>1000.0</v>
-      </c>
-      <c r="B64" s="9">
+        <v>9.9403219263764303E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="A64" s="6">
+        <v>1000</v>
+      </c>
+      <c r="B64" s="6">
         <v>0.63</v>
       </c>
       <c r="C64" s="8">
         <v>0.10138658688406471</v>
       </c>
     </row>
-    <row r="65">
-      <c r="A65" s="9">
-        <v>1100.0</v>
-      </c>
-      <c r="B65" s="9">
-        <v>0.58</v>
+    <row r="65" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="A65" s="6">
+        <v>1100</v>
+      </c>
+      <c r="B65" s="6">
+        <v>0.57999999999999996</v>
       </c>
       <c r="C65" s="8">
-        <v>0.09535953020018503</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" s="9">
-        <v>1200.0</v>
-      </c>
-      <c r="B66" s="9">
+        <v>9.5359530200185033E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="A66" s="6">
+        <v>1200</v>
+      </c>
+      <c r="B66" s="6">
         <v>0.6</v>
       </c>
       <c r="C66" s="8">
-        <v>0.0977547952787995</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" s="9">
-        <v>1250.0</v>
-      </c>
-      <c r="B67" s="9">
+        <v>9.7754795278799503E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="A67" s="6">
+        <v>1250</v>
+      </c>
+      <c r="B67" s="6">
         <v>0.53</v>
       </c>
       <c r="C67" s="8">
-        <v>0.08947424210352387</v>
+        <v>8.9474242103523866E-2</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>